<commit_message>
Fix a bug, where dynamic filter wasn't loaded and thus didn't work.
Originally NRE, then jusk commented out. The code should also deal with changed values of cells before reapply.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/AutoFilter/DynamicAutoFilter.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/AutoFilter/DynamicAutoFilter.xlsx
@@ -436,7 +436,7 @@
   </x:sheetData>
   <x:autoFilter ref="A1:A7">
     <x:filterColumn colId="0">
-      <x:dynamicFilter type="aboveAverage" val="0"/>
+      <x:dynamicFilter type="aboveAverage" val="3"/>
     </x:filterColumn>
   </x:autoFilter>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -538,7 +538,7 @@
   </x:sheetData>
   <x:autoFilter ref="A1:C7">
     <x:filterColumn colId="1">
-      <x:dynamicFilter type="belowAverage" val="0"/>
+      <x:dynamicFilter type="belowAverage" val="3"/>
     </x:filterColumn>
   </x:autoFilter>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>